<commit_message>
Created basic wizard for "Lesson" page
</commit_message>
<xml_diff>
--- a/docs/User Stories.xlsx
+++ b/docs/User Stories.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Create "Lesson" page prototype</t>
   </si>
   <si>
-    <t>Create wizard for "Lesson" page</t>
-  </si>
-  <si>
     <t>Create "Skills" page prototype</t>
   </si>
   <si>
@@ -53,6 +50,12 @@
   </si>
   <si>
     <t>Investigate mysql batabases on NodeJS</t>
+  </si>
+  <si>
+    <t>Create wizard for "Lesson" page stage #1</t>
+  </si>
+  <si>
+    <t>Create wizard for "Lesson" page stage #2</t>
   </si>
 </sst>
 </file>
@@ -413,12 +416,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF00B050"/>
+    <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,63 +438,68 @@
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>11</v>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tabs on "Lesson" page
</commit_message>
<xml_diff>
--- a/docs/User Stories.xlsx
+++ b/docs/User Stories.xlsx
@@ -81,7 +81,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +91,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,13 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -418,18 +425,17 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="83.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" customWidth="1"/>
+    <col min="3" max="4" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
@@ -473,7 +479,7 @@
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -501,6 +507,9 @@
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added "Delete file" button on tabs
</commit_message>
<xml_diff>
--- a/docs/User Stories.xlsx
+++ b/docs/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Create "Lesson" page prototype</t>
   </si>
@@ -56,13 +56,46 @@
   </si>
   <si>
     <t>Create wizard for "Lesson" page stage #2</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Install mysql server</t>
+  </si>
+  <si>
+    <t>http://dev.mysql.com/downloads/workbench/</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/mysql</t>
+  </si>
+  <si>
+    <t>Design Database architecture</t>
+  </si>
+  <si>
+    <t>Instal node-mysql package to be able to connect to the database</t>
+  </si>
+  <si>
+    <t>Design Server Architecture</t>
+  </si>
+  <si>
+    <t>Install grunt-express-server</t>
+  </si>
+  <si>
+    <t>Create cmd-runner to run development tools faster</t>
+  </si>
+  <si>
+    <t>Add "Delete file" button on tabs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +107,24 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,10 +161,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -121,8 +173,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,94 +487,145 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" customWidth="1"/>
-    <col min="3" max="4" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:3" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C21" r:id="rId1"/>
+    <hyperlink ref="C22" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>